<commit_message>
bug fix in import commodity
</commit_message>
<xml_diff>
--- a/public_html/imports/commodities-import.xlsx
+++ b/public_html/imports/commodities-import.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{493B0185-0DA8-4913-A0F8-539CE4096817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F6B3598-49A2-4950-818F-A8515D4933E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>توضیحات</t>
   </si>
@@ -49,6 +49,18 @@
   </si>
   <si>
     <t>واحد شمارش</t>
+  </si>
+  <si>
+    <t>کالا ۱</t>
+  </si>
+  <si>
+    <t>عدد</t>
+  </si>
+  <si>
+    <t>دسته بندی</t>
+  </si>
+  <si>
+    <t xml:space="preserve">سایر </t>
   </si>
 </sst>
 </file>
@@ -389,9 +401,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U1"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -431,7 +445,9 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1"/>
+      <c r="I1" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
@@ -445,6 +461,35 @@
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
     </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2">
+        <v>120</v>
+      </c>
+      <c r="E2">
+        <v>12</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>